<commit_message>
Add serialization via serialize API #208 - generation
</commit_message>
<xml_diff>
--- a/test/go/tests/serialize_test.xlsx
+++ b/test/go/tests/serialize_test.xlsx
@@ -7,20 +7,25 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Astruct" sheetId="2" r:id="rId4"/>
-    <sheet name="Bstruct" sheetId="3" r:id="rId6"/>
+    <sheet name="AstructBstruct2Use" sheetId="3" r:id="rId6"/>
+    <sheet name="AstructBstructUse" sheetId="4" r:id="rId7"/>
+    <sheet name="Bstruct" sheetId="5" r:id="rId8"/>
+    <sheet name="Dstruct" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">'Astruct'!$A$1:$V$1</definedName>
-    <definedName hidden="true" localSheetId="2" name="_xlnm._FilterDatabase">'Bstruct'!$A$1:$D$1</definedName>
+    <definedName hidden="true" localSheetId="0" name="_xlnm._FilterDatabase">'Astruct'!$A$1:$V$1</definedName>
+    <definedName hidden="true" localSheetId="1" name="_xlnm._FilterDatabase">'AstructBstruct2Use'!$A$1:$B$1</definedName>
+    <definedName hidden="true" localSheetId="2" name="_xlnm._FilterDatabase">'AstructBstructUse'!$A$1:$B$1</definedName>
+    <definedName hidden="true" localSheetId="3" name="_xlnm._FilterDatabase">'Bstruct'!$A$1:$D$1</definedName>
+    <definedName hidden="true" localSheetId="4" name="_xlnm._FilterDatabase">'Dstruct'!$A$1:$A$1</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -117,6 +122,12 @@
   <si>
     <t>B2
 B1</t>
+  </si>
+  <si>
+    <t>Bstrcut2</t>
+  </si>
+  <si>
+    <t>Bstruct2</t>
   </si>
   <si>
     <t>Floatfield2</t>
@@ -424,23 +435,12 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="true"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col customWidth="true" max="1" min="1" width="6"/>
@@ -617,6 +617,56 @@
   </sheetViews>
   <cols>
     <col customWidth="true" max="1" min="1" width="6"/>
+    <col customWidth="true" max="2" min="2" width="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="$A$1:$B$1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="6"/>
+    <col customWidth="true" max="2" min="2" width="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="$A$1:$B$1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="6"/>
     <col customWidth="true" max="2" min="2" width="12"/>
     <col customWidth="true" max="3" min="3" width="13"/>
     <col customWidth="true" max="4" min="4" width="10"/>
@@ -630,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -652,7 +702,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -667,4 +717,25 @@
   </sheetData>
   <autoFilter ref="$A$1:$D$1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="true"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col customWidth="true" max="1" min="1" width="6"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="$A$1:$A$1"/>
+</worksheet>
 </file>
</xml_diff>